<commit_message>
save after first run
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anirb\Documents\UiPath\ACME_RE_ClientSecurityHash_Bot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9947E8-D69B-4275-8285-ED00C660DC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CDB5FD-490A-44B3-9F3E-748177F4DC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -561,7 +561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1671,8 +1671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>